<commit_message>
deb int + inversement rule sort/correct
</commit_message>
<xml_diff>
--- a/resources/PACKAGES_REFRENCES/references.xlsx
+++ b/resources/PACKAGES_REFRENCES/references.xlsx
@@ -43,13 +43,13 @@
     <t xml:space="preserve">BUStools</t>
   </si>
   <si>
-    <t xml:space="preserve">Páll Melsted, Vasilis Ntranos, Lior Pachter, The barcode, UMI, set format and BUStools, Bioinformatics, Volume 35, Issue 21, 1 November 2019, Pages 4472–4473, https://doi.org/10.1093/bioinformatics/btz279</t>
+    <t xml:space="preserve">Pall Melsted, Vasilis Ntranos, Lior Pachter, The barcode, UMI, set format and BUStools, Bioinformatics, Volume 35, Issue 21, 1 November 2019, Pages 4472-4473, https://doi.org/10.1093/bioinformatics/btz279</t>
   </si>
   <si>
     <t xml:space="preserve">Cerebro</t>
   </si>
   <si>
-    <t xml:space="preserve">Roman Hillje, Pier Giuseppe Pelicci, Lucilla Luzi, Cerebro: interactive visualization of scRNA-seq data, Bioinformatics, Volume 36, Issue 7, 1 April 2020, Pages 2311–2313, https://doi.org/10.1093/bioinformatics/btz877</t>
+    <t xml:space="preserve">Roman Hillje, Pier Giuseppe Pelicci, Lucilla Luzi, Cerebro: interactive visualization of scRNA-seq data, Bioinformatics, Volume 36, Issue 7, 1 April 2020, Pages 2311-2313, https://doi.org/10.1093/bioinformatics/btz877</t>
   </si>
   <si>
     <t xml:space="preserve">ClustifyR</t>
@@ -80,19 +80,19 @@
     <t xml:space="preserve">Harmony</t>
   </si>
   <si>
-    <t xml:space="preserve">Korsunsky, I., Millard, N., Fan, J. et al. Fast, sensitive and accurate integration of single-cell data with Harmony. Nat Methods 16, 1289–1296 (2019). https://doi.org/10.1038/s41592-019-0619-0</t>
+    <t xml:space="preserve">Korsunsky, I., Millard, N., Fan, J. et al. Fast, sensitive and accurate integration of single-cell data with Harmony. Nat Methods 16, 1289-1296 (2019). https://doi.org/10.1038/s41592-019-0619-0</t>
   </si>
   <si>
     <t xml:space="preserve">kallisto</t>
   </si>
   <si>
-    <t xml:space="preserve">Nicolas L Bray, Harold Pimentel, Páll Melsted and Lior Pachter, Near-optimal probabilistic RNA-seq quantification, Nature Biotechnology 34, 525–527 (2016), doi:10.1038/nbt.3519</t>
+    <t xml:space="preserve">Nicolas L Bray, Harold Pimentel, Pall Melsted and Lior Pachter, Near-optimal probabilistic RNA-seq quantification, Nature Biotechnology 34, 525-527 (2016), doi:10.1038/nbt.3519</t>
   </si>
   <si>
     <t xml:space="preserve">kb-python</t>
   </si>
   <si>
-    <t xml:space="preserve">Bray, N. L., Pimentel, H., Melsted, P., &amp; Pachter, L. (2016). Near-optimal probabilistic RNA-seq quantification. Nature biotechnology, 34(5), 525. ; Melsted, P., Booeshaghi, A. S., Gao, F., da Veiga Beltrame, E., Lu, L., Hjorleifsson, K. E., Gehring, J., &amp; Pachter, L. (2019). Modular and efficient pre-processing of single-cell RNA-seq. BioRxiv, 673285.</t>
+    <t xml:space="preserve">Bray, N. L., Pimentel, H., Melsted, P., &amp; Pachter, L. (2016). Near-optimal probabilistic RNA-seq quantification. Nature biotechnology, 34(5), 525 ; Melsted, P., Booeshaghi, A. S., Gao, F., da Veiga Beltrame, E., Lu, L., Hjorleifsson, K. E., Gehring, J., &amp; Pachter, L. (2019). Modular and efficient pre-processing of single-cell RNA-seq. BioRxiv, 673285.</t>
   </si>
   <si>
     <t xml:space="preserve">Liger</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">Seurat</t>
   </si>
   <si>
-    <t xml:space="preserve">Butler, A., Hoffman, P., Smibert, P., Papalexi, E. &amp; Satija, R. Integrating single-cell transcriptomic data across different conditions, technologies, and species. Nat. Biotechnol. 36, 411–420 (2018)</t>
+    <t xml:space="preserve">Butler, A., Hoffman, P., Smibert, P., Papalexi, E. &amp; Satija, R. Integrating single-cell transcriptomic data across different conditions, technologies, and species. Nat. Biotechnol. 36, 411-420 (2018)</t>
   </si>
   <si>
     <t xml:space="preserve">SingleR</t>
@@ -250,14 +250,14 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="2" sqref="B5 B10 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="333.09693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="326.005102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
orthograph correction of packages references publications
</commit_message>
<xml_diff>
--- a/resources/PACKAGES_REFRENCES/references.xlsx
+++ b/resources/PACKAGES_REFRENCES/references.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="references" sheetId="1" state="visible" r:id="rId2"/>
@@ -67,8 +67,7 @@
     <t xml:space="preserve">dropletUtils</t>
   </si>
   <si>
-    <t xml:space="preserve">Lun ATL, Riesenfeld S, Andrews T, Dao T, Gomes T, participants in the 1st Human Cell Atlas Jamboree, Marioni JC (2019). EmptyDrops: distinguishing cells from empty droplets in droplet-based single-cell RNA sequencing data. Genome Biol., 20, 63. doi: 10.1186/s13059-019-1662-y. 
-Griffiths JA, Richard AC, Bach K, Lun ATL, Marioni JC (2018). Detection and removal of barcode swapping in single-cell RNA-seq data. Nat. Commun., 9(1), 2667. doi: 10.1038/s41467-018-05083-x. </t>
+    <t xml:space="preserve">Lun ATL, Riesenfeld S, Andrews T, Dao T, Gomes T, participants in the 1st Human Cell Atlas Jamboree, Marioni JC (2019). EmptyDrops: distinguishing cells from empty droplets in droplet-based single-cell RNA sequencing data. Genome Biol., 20, 63. doi: 10.1186/s13059-019-1662-y. ; Griffiths JA, Richard AC, Bach K, Lun ATL, Marioni JC (2018). Detection and removal of barcode swapping in single-cell RNA-seq data. Nat. Commun., 9(1), 2667. doi: 10.1038/s41467-018-05083-x. </t>
   </si>
   <si>
     <t xml:space="preserve">fastq-screen</t>
@@ -250,14 +249,14 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="2" sqref="B5 B10 B7"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="326.005102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="322.494897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>